<commit_message>
working on random forest
</commit_message>
<xml_diff>
--- a/data/Data LA Study 20211208.xlsx
+++ b/data/Data LA Study 20211208.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhmockrin\Box\_Workspace\Proj_GitHub\la_wui_2112\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23DA495-6A46-40D1-BE71-62CA45AB270F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28031BE0-B0A4-4562-B11B-267833EDA221}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_20211019_RForest" sheetId="10" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="crosswalk_research_guidelines_d" sheetId="8" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data_20211019_RForest!$B$79:$B$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data_20211019_RForest!$A$1:$K$78</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">data_checklist_190514!$A$2:$AE$92</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Data_request_190524!$A$2:$AC$56</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Price_2021 categories'!$A$2:$E$91</definedName>
@@ -1747,15 +1747,6 @@
     <t>Do trees overhang building (binary)</t>
   </si>
   <si>
-    <t>Distance to nearest shrub (units?)</t>
-  </si>
-  <si>
-    <t>Distance to nearest tree (units?)</t>
-  </si>
-  <si>
-    <t>Average height of trees overhanging building (units)</t>
-  </si>
-  <si>
     <t>Percent of building with trees over top</t>
   </si>
   <si>
@@ -1825,9 +1816,6 @@
     <t>Eaves (enclosed, unenclosed, unknown, no eaves)</t>
   </si>
   <si>
-    <t>Building area (units?)</t>
-  </si>
-  <si>
     <t>Buildings destroyed (major/destroyed) vs. surviving (no damage, affected, minor)</t>
   </si>
   <si>
@@ -1837,9 +1825,6 @@
     <t>damage_binary</t>
   </si>
   <si>
-    <t>Distance to nearest destroyed building (units?)</t>
-  </si>
-  <si>
     <t>Interpolated housing density based on a 1-km search radius NOTE - housing? Structure?</t>
   </si>
   <si>
@@ -1849,18 +1834,6 @@
     <t xml:space="preserve">Percentage slope, 100 m around building, derived from a 30 m digital elevation model </t>
   </si>
   <si>
-    <t>Elevation, 30 m around building, derived from a 30 m digital elevation model UNIT</t>
-  </si>
-  <si>
-    <t>Elevation, 100 m around building, derived from a 30 m digital elevation model UNIT</t>
-  </si>
-  <si>
-    <t>Euclidian distance to any road (major and minor)- UNIT</t>
-  </si>
-  <si>
-    <t>Euclidian distance to major road-UNIT</t>
-  </si>
-  <si>
     <t>Aspect, 100 m around building, derived from a 30 m digital elevation model</t>
   </si>
   <si>
@@ -1969,7 +1942,34 @@
     <t>Percent water land cover, 300 m around building</t>
   </si>
   <si>
-    <t>Parcel area UNITS</t>
+    <t>Building area (UNITS)</t>
+  </si>
+  <si>
+    <t>Distance to nearest shrub (UNITS)</t>
+  </si>
+  <si>
+    <t>Distance to nearest tree (UNITS)</t>
+  </si>
+  <si>
+    <t>Average height of trees overhanging building (UNITS)</t>
+  </si>
+  <si>
+    <t>Parcel area (UNITS)</t>
+  </si>
+  <si>
+    <t>Euclidian distance to any road (major and minor)- (UNITS)</t>
+  </si>
+  <si>
+    <t>Euclidian distance to major road (UNITS)</t>
+  </si>
+  <si>
+    <t>Distance to nearest destroyed building (UNITS)</t>
+  </si>
+  <si>
+    <t>Elevation, 100 m around building, derived from a 30 m digital elevation model UNITS</t>
+  </si>
+  <si>
+    <t>Elevation, 30 m around building, derived from a 30 m digital elevation model UNITS</t>
   </si>
 </sst>
 </file>
@@ -1985,42 +1985,50 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2219,7 +2227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2348,6 +2356,7 @@
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2662,14 +2671,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E470F27-90FE-46CE-BDA9-72D77DAC3EC2}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2677,7 +2686,7 @@
     <col min="1" max="1" width="9.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" style="53" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="4" customWidth="1"/>
     <col min="5" max="5" width="97" style="62" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" style="4"/>
     <col min="7" max="7" width="29.5703125" style="4" customWidth="1"/>
@@ -2717,7 +2726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="55" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="55" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
         <v>461</v>
       </c>
@@ -2728,10 +2737,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="55" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="E2" s="55" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="F2" s="54" t="s">
         <v>11</v>
@@ -2755,7 +2764,7 @@
         <v>485</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>587</v>
+        <v>626</v>
       </c>
       <c r="F3" s="54" t="s">
         <v>11</v>
@@ -2767,7 +2776,7 @@
       <c r="I3" s="54"/>
       <c r="J3" s="54"/>
     </row>
-    <row r="4" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="52">
         <v>2</v>
       </c>
@@ -2781,7 +2790,7 @@
         <v>486</v>
       </c>
       <c r="E4" s="62" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="F4" s="54" t="s">
         <v>11</v>
@@ -2795,7 +2804,7 @@
       </c>
       <c r="J4" s="54"/>
     </row>
-    <row r="5" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="52">
         <v>3</v>
       </c>
@@ -2809,7 +2818,7 @@
         <v>487</v>
       </c>
       <c r="E5" s="62" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="F5" s="54" t="s">
         <v>11</v>
@@ -2821,7 +2830,7 @@
       <c r="I5" s="54"/>
       <c r="J5" s="54"/>
     </row>
-    <row r="6" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="52">
         <v>4</v>
       </c>
@@ -2835,7 +2844,7 @@
         <v>488</v>
       </c>
       <c r="E6" s="62" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="F6" s="54" t="s">
         <v>11</v>
@@ -2847,7 +2856,7 @@
       <c r="I6" s="54"/>
       <c r="J6" s="54"/>
     </row>
-    <row r="7" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="52">
         <v>5</v>
       </c>
@@ -2861,7 +2870,7 @@
         <v>489</v>
       </c>
       <c r="E7" s="62" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="F7" s="54" t="s">
         <v>11</v>
@@ -2873,7 +2882,7 @@
       <c r="I7" s="54"/>
       <c r="J7" s="54"/>
     </row>
-    <row r="8" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="52">
         <v>6</v>
       </c>
@@ -2887,7 +2896,7 @@
         <v>490</v>
       </c>
       <c r="E8" s="62" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="F8" s="54" t="s">
         <v>11</v>
@@ -2899,7 +2908,7 @@
       <c r="I8" s="54"/>
       <c r="J8" s="54"/>
     </row>
-    <row r="9" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="52">
         <v>7</v>
       </c>
@@ -2913,7 +2922,7 @@
         <v>491</v>
       </c>
       <c r="E9" s="62" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="F9" s="54" t="s">
         <v>11</v>
@@ -2925,7 +2934,7 @@
       <c r="I9" s="54"/>
       <c r="J9" s="54"/>
     </row>
-    <row r="10" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="52">
         <v>8</v>
       </c>
@@ -2939,7 +2948,7 @@
         <v>492</v>
       </c>
       <c r="E10" s="62" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="F10" s="54" t="s">
         <v>11</v>
@@ -2951,7 +2960,7 @@
       <c r="I10" s="54"/>
       <c r="J10" s="54"/>
     </row>
-    <row r="11" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="52">
         <v>9</v>
       </c>
@@ -2965,7 +2974,7 @@
         <v>493</v>
       </c>
       <c r="E11" s="62" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="F11" s="54" t="s">
         <v>11</v>
@@ -2977,7 +2986,7 @@
       <c r="I11" s="54"/>
       <c r="J11" s="54"/>
     </row>
-    <row r="12" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="52">
         <v>10</v>
       </c>
@@ -2991,7 +3000,7 @@
         <v>494</v>
       </c>
       <c r="E12" s="62" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F12" s="54" t="s">
         <v>11</v>
@@ -3003,7 +3012,7 @@
       <c r="I12" s="54"/>
       <c r="J12" s="54"/>
     </row>
-    <row r="13" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="52">
         <v>11</v>
       </c>
@@ -3017,7 +3026,7 @@
         <v>495</v>
       </c>
       <c r="E13" s="62" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="F13" s="54" t="s">
         <v>11</v>
@@ -3029,7 +3038,7 @@
       <c r="I13" s="54"/>
       <c r="J13" s="54"/>
     </row>
-    <row r="14" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="52">
         <v>12</v>
       </c>
@@ -3043,7 +3052,7 @@
         <v>496</v>
       </c>
       <c r="E14" s="62" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="F14" s="54" t="s">
         <v>11</v>
@@ -3055,7 +3064,7 @@
       <c r="I14" s="54"/>
       <c r="J14" s="54"/>
     </row>
-    <row r="15" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="52">
         <v>13</v>
       </c>
@@ -3083,7 +3092,7 @@
       </c>
       <c r="J15" s="56"/>
     </row>
-    <row r="16" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="52">
         <v>14</v>
       </c>
@@ -3112,7 +3121,7 @@
       <c r="J16" s="54"/>
       <c r="K16" s="54"/>
     </row>
-    <row r="17" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="52">
         <v>15</v>
       </c>
@@ -3152,8 +3161,8 @@
       <c r="D18" s="57" t="s">
         <v>502</v>
       </c>
-      <c r="E18" s="62" t="s">
-        <v>563</v>
+      <c r="E18" s="66" t="s">
+        <v>629</v>
       </c>
       <c r="F18" s="54" t="s">
         <v>11</v>
@@ -3166,7 +3175,7 @@
       <c r="J18" s="54"/>
       <c r="K18" s="54"/>
     </row>
-    <row r="19" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="52">
         <v>16</v>
       </c>
@@ -3180,7 +3189,7 @@
         <v>503</v>
       </c>
       <c r="E19" s="62" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="F19" s="54" t="s">
         <v>11</v>
@@ -3208,8 +3217,8 @@
       <c r="D20" s="57" t="s">
         <v>500</v>
       </c>
-      <c r="E20" s="62" t="s">
-        <v>561</v>
+      <c r="E20" s="66" t="s">
+        <v>627</v>
       </c>
       <c r="F20" s="54" t="s">
         <v>11</v>
@@ -3235,8 +3244,8 @@
       <c r="D21" s="57" t="s">
         <v>501</v>
       </c>
-      <c r="E21" s="62" t="s">
-        <v>562</v>
+      <c r="E21" s="66" t="s">
+        <v>628</v>
       </c>
       <c r="F21" s="54" t="s">
         <v>11</v>
@@ -3249,7 +3258,7 @@
       <c r="J21" s="54"/>
       <c r="K21" s="54"/>
     </row>
-    <row r="22" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="52">
         <v>20</v>
       </c>
@@ -3263,7 +3272,7 @@
         <v>504</v>
       </c>
       <c r="E22" s="62" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="F22" s="54" t="s">
         <v>41</v>
@@ -3278,7 +3287,7 @@
       <c r="J22" s="54"/>
       <c r="K22" s="54"/>
     </row>
-    <row r="23" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="52">
         <v>21</v>
       </c>
@@ -3292,7 +3301,7 @@
         <v>505</v>
       </c>
       <c r="E23" s="62" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="F23" s="54" t="s">
         <v>41</v>
@@ -3305,7 +3314,7 @@
       <c r="J23" s="54"/>
       <c r="K23" s="54"/>
     </row>
-    <row r="24" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="52">
         <v>22</v>
       </c>
@@ -3319,7 +3328,7 @@
         <v>506</v>
       </c>
       <c r="E24" s="62" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="F24" s="54" t="s">
         <v>41</v>
@@ -3332,7 +3341,7 @@
       <c r="J24" s="54"/>
       <c r="K24" s="54"/>
     </row>
-    <row r="25" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="52">
         <v>23</v>
       </c>
@@ -3346,7 +3355,7 @@
         <v>507</v>
       </c>
       <c r="E25" s="62" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="F25" s="54" t="s">
         <v>41</v>
@@ -3359,7 +3368,7 @@
       <c r="J25" s="54"/>
       <c r="K25" s="54"/>
     </row>
-    <row r="26" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="52">
         <v>24</v>
       </c>
@@ -3373,7 +3382,7 @@
         <v>508</v>
       </c>
       <c r="E26" s="62" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="F26" s="54" t="s">
         <v>41</v>
@@ -3386,7 +3395,7 @@
       <c r="J26" s="54"/>
       <c r="K26" s="54"/>
     </row>
-    <row r="27" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="52">
         <v>25</v>
       </c>
@@ -3400,7 +3409,7 @@
         <v>509</v>
       </c>
       <c r="E27" s="62" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="F27" s="54" t="s">
         <v>41</v>
@@ -3413,7 +3422,7 @@
       <c r="J27" s="54"/>
       <c r="K27" s="54"/>
     </row>
-    <row r="28" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="52">
         <v>26</v>
       </c>
@@ -3427,7 +3436,7 @@
         <v>510</v>
       </c>
       <c r="E28" s="62" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="F28" s="54" t="s">
         <v>41</v>
@@ -3442,7 +3451,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="52">
         <v>27</v>
       </c>
@@ -3456,7 +3465,7 @@
         <v>511</v>
       </c>
       <c r="E29" s="62" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="F29" s="54" t="s">
         <v>41</v>
@@ -3471,7 +3480,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="52">
         <v>28</v>
       </c>
@@ -3485,7 +3494,7 @@
         <v>512</v>
       </c>
       <c r="E30" s="62" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="F30" s="54" t="s">
         <v>41</v>
@@ -3497,7 +3506,7 @@
       <c r="I30" s="54"/>
       <c r="J30" s="54"/>
     </row>
-    <row r="31" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="52">
         <v>29</v>
       </c>
@@ -3511,7 +3520,7 @@
         <v>513</v>
       </c>
       <c r="E31" s="62" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F31" s="54" t="s">
         <v>41</v>
@@ -3535,8 +3544,8 @@
       <c r="D32" s="57" t="s">
         <v>514</v>
       </c>
-      <c r="E32" s="62" t="s">
-        <v>591</v>
+      <c r="E32" s="66" t="s">
+        <v>633</v>
       </c>
       <c r="F32" s="54" t="s">
         <v>11</v>
@@ -3552,7 +3561,7 @@
       </c>
       <c r="K32" s="54"/>
     </row>
-    <row r="33" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="52">
         <v>31</v>
       </c>
@@ -3566,7 +3575,7 @@
         <v>515</v>
       </c>
       <c r="E33" s="62" t="s">
-        <v>603</v>
+        <v>594</v>
       </c>
       <c r="F33" s="54" t="s">
         <v>11</v>
@@ -3579,7 +3588,7 @@
       </c>
       <c r="K33" s="54"/>
     </row>
-    <row r="34" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="52">
         <v>32</v>
       </c>
@@ -3593,7 +3602,7 @@
         <v>516</v>
       </c>
       <c r="E34" s="62" t="s">
-        <v>604</v>
+        <v>595</v>
       </c>
       <c r="F34" s="54" t="s">
         <v>11</v>
@@ -3604,7 +3613,7 @@
       <c r="H34" s="54"/>
       <c r="K34" s="54"/>
     </row>
-    <row r="35" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="52">
         <v>33</v>
       </c>
@@ -3618,7 +3627,7 @@
         <v>517</v>
       </c>
       <c r="E35" s="62" t="s">
-        <v>605</v>
+        <v>596</v>
       </c>
       <c r="F35" s="54" t="s">
         <v>11</v>
@@ -3629,7 +3638,7 @@
       <c r="H35" s="54"/>
       <c r="K35" s="54"/>
     </row>
-    <row r="36" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="52">
         <v>34</v>
       </c>
@@ -3643,7 +3652,7 @@
         <v>518</v>
       </c>
       <c r="E36" s="62" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
       <c r="F36" s="54" t="s">
         <v>11</v>
@@ -3654,7 +3663,7 @@
       <c r="H36" s="54"/>
       <c r="K36" s="54"/>
     </row>
-    <row r="37" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="52">
         <v>35</v>
       </c>
@@ -3668,7 +3677,7 @@
         <v>519</v>
       </c>
       <c r="E37" s="62" t="s">
-        <v>607</v>
+        <v>598</v>
       </c>
       <c r="F37" s="54" t="s">
         <v>11</v>
@@ -3679,7 +3688,7 @@
       <c r="H37" s="54"/>
       <c r="K37" s="54"/>
     </row>
-    <row r="38" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="52">
         <v>36</v>
       </c>
@@ -3693,7 +3702,7 @@
         <v>520</v>
       </c>
       <c r="E38" s="62" t="s">
-        <v>608</v>
+        <v>599</v>
       </c>
       <c r="F38" s="54" t="s">
         <v>11</v>
@@ -3704,7 +3713,7 @@
       <c r="H38" s="54"/>
       <c r="K38" s="54"/>
     </row>
-    <row r="39" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="52">
         <v>37</v>
       </c>
@@ -3718,7 +3727,7 @@
         <v>521</v>
       </c>
       <c r="E39" s="62" t="s">
-        <v>609</v>
+        <v>600</v>
       </c>
       <c r="F39" s="54" t="s">
         <v>11</v>
@@ -3729,7 +3738,7 @@
       <c r="H39" s="54"/>
       <c r="K39" s="54"/>
     </row>
-    <row r="40" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="52">
         <v>38</v>
       </c>
@@ -3743,7 +3752,7 @@
         <v>522</v>
       </c>
       <c r="E40" s="62" t="s">
-        <v>610</v>
+        <v>601</v>
       </c>
       <c r="F40" s="54" t="s">
         <v>11</v>
@@ -3754,7 +3763,7 @@
       <c r="H40" s="54"/>
       <c r="K40" s="54"/>
     </row>
-    <row r="41" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="52">
         <v>39</v>
       </c>
@@ -3768,7 +3777,7 @@
         <v>523</v>
       </c>
       <c r="E41" s="62" t="s">
-        <v>611</v>
+        <v>602</v>
       </c>
       <c r="F41" s="54" t="s">
         <v>11</v>
@@ -3779,7 +3788,7 @@
       <c r="H41" s="54"/>
       <c r="K41" s="54"/>
     </row>
-    <row r="42" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="52">
         <v>40</v>
       </c>
@@ -3793,7 +3802,7 @@
         <v>524</v>
       </c>
       <c r="E42" s="62" t="s">
-        <v>612</v>
+        <v>603</v>
       </c>
       <c r="F42" s="54" t="s">
         <v>11</v>
@@ -3804,7 +3813,7 @@
       <c r="H42" s="54"/>
       <c r="K42" s="54"/>
     </row>
-    <row r="43" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="52">
         <v>41</v>
       </c>
@@ -3818,7 +3827,7 @@
         <v>525</v>
       </c>
       <c r="E43" s="62" t="s">
-        <v>613</v>
+        <v>604</v>
       </c>
       <c r="F43" s="54" t="s">
         <v>11</v>
@@ -3829,7 +3838,7 @@
       <c r="H43" s="54"/>
       <c r="K43" s="54"/>
     </row>
-    <row r="44" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="52">
         <v>42</v>
       </c>
@@ -3843,7 +3852,7 @@
         <v>526</v>
       </c>
       <c r="E44" s="62" t="s">
-        <v>614</v>
+        <v>605</v>
       </c>
       <c r="F44" s="54" t="s">
         <v>11</v>
@@ -3855,7 +3864,7 @@
       <c r="J44" s="54"/>
       <c r="K44" s="54"/>
     </row>
-    <row r="45" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="52">
         <v>43</v>
       </c>
@@ -3869,7 +3878,7 @@
         <v>527</v>
       </c>
       <c r="E45" s="62" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="F45" s="54" t="s">
         <v>11</v>
@@ -3882,7 +3891,7 @@
       <c r="J45" s="54"/>
       <c r="K45" s="54"/>
     </row>
-    <row r="46" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="52">
         <v>44</v>
       </c>
@@ -3896,7 +3905,7 @@
         <v>528</v>
       </c>
       <c r="E46" s="62" t="s">
-        <v>616</v>
+        <v>607</v>
       </c>
       <c r="F46" s="54" t="s">
         <v>11</v>
@@ -3909,7 +3918,7 @@
       <c r="J46" s="54"/>
       <c r="K46" s="54"/>
     </row>
-    <row r="47" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="52">
         <v>45</v>
       </c>
@@ -3923,7 +3932,7 @@
         <v>529</v>
       </c>
       <c r="E47" s="62" t="s">
-        <v>617</v>
+        <v>608</v>
       </c>
       <c r="F47" s="54" t="s">
         <v>11</v>
@@ -3936,7 +3945,7 @@
       <c r="J47" s="54"/>
       <c r="K47" s="54"/>
     </row>
-    <row r="48" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="52">
         <v>46</v>
       </c>
@@ -3950,7 +3959,7 @@
         <v>530</v>
       </c>
       <c r="E48" s="62" t="s">
-        <v>618</v>
+        <v>609</v>
       </c>
       <c r="F48" s="54" t="s">
         <v>11</v>
@@ -3963,7 +3972,7 @@
       <c r="J48" s="54"/>
       <c r="K48" s="54"/>
     </row>
-    <row r="49" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="52">
         <v>47</v>
       </c>
@@ -3977,7 +3986,7 @@
         <v>531</v>
       </c>
       <c r="E49" s="62" t="s">
-        <v>619</v>
+        <v>610</v>
       </c>
       <c r="F49" s="54" t="s">
         <v>11</v>
@@ -3990,7 +3999,7 @@
       <c r="J49" s="54"/>
       <c r="K49" s="54"/>
     </row>
-    <row r="50" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="52">
         <v>48</v>
       </c>
@@ -4004,7 +4013,7 @@
         <v>532</v>
       </c>
       <c r="E50" s="62" t="s">
-        <v>620</v>
+        <v>611</v>
       </c>
       <c r="F50" s="54" t="s">
         <v>11</v>
@@ -4017,7 +4026,7 @@
       <c r="J50" s="54"/>
       <c r="K50" s="54"/>
     </row>
-    <row r="51" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="52">
         <v>49</v>
       </c>
@@ -4031,7 +4040,7 @@
         <v>533</v>
       </c>
       <c r="E51" s="62" t="s">
-        <v>621</v>
+        <v>612</v>
       </c>
       <c r="F51" s="54" t="s">
         <v>11</v>
@@ -4044,7 +4053,7 @@
       <c r="J51" s="54"/>
       <c r="K51" s="54"/>
     </row>
-    <row r="52" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="52">
         <v>50</v>
       </c>
@@ -4058,7 +4067,7 @@
         <v>534</v>
       </c>
       <c r="E52" s="62" t="s">
-        <v>622</v>
+        <v>613</v>
       </c>
       <c r="F52" s="54" t="s">
         <v>11</v>
@@ -4071,7 +4080,7 @@
       <c r="J52" s="54"/>
       <c r="K52" s="54"/>
     </row>
-    <row r="53" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="52">
         <v>51</v>
       </c>
@@ -4085,7 +4094,7 @@
         <v>535</v>
       </c>
       <c r="E53" s="62" t="s">
-        <v>623</v>
+        <v>614</v>
       </c>
       <c r="F53" s="54" t="s">
         <v>11</v>
@@ -4098,7 +4107,7 @@
       <c r="J53" s="54"/>
       <c r="K53" s="54"/>
     </row>
-    <row r="54" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="52">
         <v>52</v>
       </c>
@@ -4112,7 +4121,7 @@
         <v>536</v>
       </c>
       <c r="E54" s="62" t="s">
-        <v>624</v>
+        <v>615</v>
       </c>
       <c r="F54" s="54" t="s">
         <v>11</v>
@@ -4125,7 +4134,7 @@
       <c r="J54" s="54"/>
       <c r="K54" s="54"/>
     </row>
-    <row r="55" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="52">
         <v>53</v>
       </c>
@@ -4139,7 +4148,7 @@
         <v>537</v>
       </c>
       <c r="E55" s="62" t="s">
-        <v>625</v>
+        <v>616</v>
       </c>
       <c r="F55" s="54" t="s">
         <v>11</v>
@@ -4152,7 +4161,7 @@
       <c r="J55" s="54"/>
       <c r="K55" s="54"/>
     </row>
-    <row r="56" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="52">
         <v>54</v>
       </c>
@@ -4166,7 +4175,7 @@
         <v>538</v>
       </c>
       <c r="E56" s="62" t="s">
-        <v>626</v>
+        <v>617</v>
       </c>
       <c r="F56" s="54" t="s">
         <v>11</v>
@@ -4179,7 +4188,7 @@
       <c r="J56" s="54"/>
       <c r="K56" s="54"/>
     </row>
-    <row r="57" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="52">
         <v>55</v>
       </c>
@@ -4193,7 +4202,7 @@
         <v>539</v>
       </c>
       <c r="E57" s="62" t="s">
-        <v>627</v>
+        <v>618</v>
       </c>
       <c r="F57" s="54" t="s">
         <v>11</v>
@@ -4206,7 +4215,7 @@
       <c r="J57" s="54"/>
       <c r="K57" s="54"/>
     </row>
-    <row r="58" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="52">
         <v>56</v>
       </c>
@@ -4220,7 +4229,7 @@
         <v>540</v>
       </c>
       <c r="E58" s="62" t="s">
-        <v>628</v>
+        <v>619</v>
       </c>
       <c r="F58" s="54" t="s">
         <v>11</v>
@@ -4233,7 +4242,7 @@
       <c r="J58" s="54"/>
       <c r="K58" s="54"/>
     </row>
-    <row r="59" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="52">
         <v>57</v>
       </c>
@@ -4247,7 +4256,7 @@
         <v>541</v>
       </c>
       <c r="E59" s="62" t="s">
-        <v>629</v>
+        <v>620</v>
       </c>
       <c r="F59" s="54" t="s">
         <v>11</v>
@@ -4260,7 +4269,7 @@
       <c r="J59" s="54"/>
       <c r="K59" s="54"/>
     </row>
-    <row r="60" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="52">
         <v>58</v>
       </c>
@@ -4274,7 +4283,7 @@
         <v>542</v>
       </c>
       <c r="E60" s="62" t="s">
-        <v>630</v>
+        <v>621</v>
       </c>
       <c r="F60" s="54" t="s">
         <v>11</v>
@@ -4287,7 +4296,7 @@
       <c r="J60" s="54"/>
       <c r="K60" s="54"/>
     </row>
-    <row r="61" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="52">
         <v>59</v>
       </c>
@@ -4301,7 +4310,7 @@
         <v>543</v>
       </c>
       <c r="E61" s="62" t="s">
-        <v>631</v>
+        <v>622</v>
       </c>
       <c r="F61" s="54" t="s">
         <v>11</v>
@@ -4314,7 +4323,7 @@
       <c r="J61" s="54"/>
       <c r="K61" s="54"/>
     </row>
-    <row r="62" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="52">
         <v>60</v>
       </c>
@@ -4328,7 +4337,7 @@
         <v>544</v>
       </c>
       <c r="E62" s="62" t="s">
-        <v>632</v>
+        <v>623</v>
       </c>
       <c r="F62" s="54" t="s">
         <v>11</v>
@@ -4341,7 +4350,7 @@
       <c r="J62" s="54"/>
       <c r="K62" s="54"/>
     </row>
-    <row r="63" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="52">
         <v>61</v>
       </c>
@@ -4355,7 +4364,7 @@
         <v>545</v>
       </c>
       <c r="E63" s="62" t="s">
-        <v>633</v>
+        <v>624</v>
       </c>
       <c r="F63" s="54" t="s">
         <v>11</v>
@@ -4368,7 +4377,7 @@
       <c r="J63" s="54"/>
       <c r="K63" s="54"/>
     </row>
-    <row r="64" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="52">
         <v>62</v>
       </c>
@@ -4382,7 +4391,7 @@
         <v>546</v>
       </c>
       <c r="E64" s="62" t="s">
-        <v>634</v>
+        <v>625</v>
       </c>
       <c r="F64" s="54" t="s">
         <v>11</v>
@@ -4408,8 +4417,8 @@
       <c r="D65" s="57" t="s">
         <v>547</v>
       </c>
-      <c r="E65" s="62" t="s">
-        <v>635</v>
+      <c r="E65" s="66" t="s">
+        <v>630</v>
       </c>
       <c r="F65" s="54" t="s">
         <v>41</v>
@@ -4434,8 +4443,8 @@
       <c r="D66" s="57" t="s">
         <v>548</v>
       </c>
-      <c r="E66" s="62" t="s">
-        <v>592</v>
+      <c r="E66" s="66" t="s">
+        <v>587</v>
       </c>
       <c r="F66" s="54" t="s">
         <v>55</v>
@@ -4462,8 +4471,8 @@
       <c r="D67" s="57" t="s">
         <v>549</v>
       </c>
-      <c r="E67" s="62" t="s">
-        <v>597</v>
+      <c r="E67" s="66" t="s">
+        <v>631</v>
       </c>
       <c r="F67" s="54" t="s">
         <v>55</v>
@@ -4488,8 +4497,8 @@
       <c r="D68" s="57" t="s">
         <v>550</v>
       </c>
-      <c r="E68" s="62" t="s">
-        <v>598</v>
+      <c r="E68" s="66" t="s">
+        <v>632</v>
       </c>
       <c r="F68" s="54" t="s">
         <v>55</v>
@@ -4500,7 +4509,7 @@
       <c r="H68" s="54"/>
       <c r="K68" s="54"/>
     </row>
-    <row r="69" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="52">
         <v>67</v>
       </c>
@@ -4514,7 +4523,7 @@
         <v>551</v>
       </c>
       <c r="E69" s="55" t="s">
-        <v>599</v>
+        <v>590</v>
       </c>
       <c r="F69" s="54" t="s">
         <v>11</v>
@@ -4532,7 +4541,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="52">
         <v>68</v>
       </c>
@@ -4546,7 +4555,7 @@
         <v>552</v>
       </c>
       <c r="E70" s="55" t="s">
-        <v>600</v>
+        <v>591</v>
       </c>
       <c r="F70" s="54" t="s">
         <v>11</v>
@@ -4577,8 +4586,8 @@
       <c r="D71" s="55" t="s">
         <v>553</v>
       </c>
-      <c r="E71" s="55" t="s">
-        <v>596</v>
+      <c r="E71" s="66" t="s">
+        <v>634</v>
       </c>
       <c r="F71" s="54" t="s">
         <v>11</v>
@@ -4609,8 +4618,8 @@
       <c r="D72" s="55" t="s">
         <v>554</v>
       </c>
-      <c r="E72" s="55" t="s">
-        <v>595</v>
+      <c r="E72" s="66" t="s">
+        <v>635</v>
       </c>
       <c r="F72" s="54" t="s">
         <v>11</v>
@@ -4628,7 +4637,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="52">
         <v>71</v>
       </c>
@@ -4642,7 +4651,7 @@
         <v>555</v>
       </c>
       <c r="E73" s="55" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="F73" s="54" t="s">
         <v>11</v>
@@ -4658,7 +4667,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="52">
         <v>72</v>
       </c>
@@ -4672,7 +4681,7 @@
         <v>556</v>
       </c>
       <c r="E74" s="55" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="F74" s="54" t="s">
         <v>11</v>
@@ -4687,7 +4696,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="52" t="s">
         <v>461</v>
       </c>
@@ -4701,7 +4710,7 @@
         <v>467</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="F75" s="54" t="s">
         <v>41</v>
@@ -4714,7 +4723,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="76" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="52" t="s">
         <v>461</v>
       </c>
@@ -4728,7 +4737,7 @@
         <v>466</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="F76" s="54" t="s">
         <v>41</v>
@@ -4741,7 +4750,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="52" t="s">
         <v>461</v>
       </c>
@@ -4755,7 +4764,7 @@
         <v>465</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
       <c r="F77" s="54" t="s">
         <v>41</v>
@@ -4768,7 +4777,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="52" t="s">
         <v>461</v>
       </c>
@@ -4782,7 +4791,7 @@
         <v>464</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>602</v>
+        <v>593</v>
       </c>
       <c r="F78" s="54" t="s">
         <v>41</v>
@@ -11321,6 +11330,14 @@
       <c r="E1015" s="9"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K78" xr:uid="{1E3BF0EA-EC3D-444C-9AE7-3F99453DC04F}">
+    <filterColumn colId="4">
+      <customFilters>
+        <customFilter val="*UNIT*"/>
+        <customFilter val="*NOTE*"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A13:K21">
     <sortCondition ref="A13:A21"/>
   </sortState>
@@ -29331,7 +29348,9 @@
   </sheetPr>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -29593,10 +29612,10 @@
   <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -30447,11 +30466,11 @@
   </sheetPr>
   <dimension ref="A1:AE1082"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
working on random forest w DINS
</commit_message>
<xml_diff>
--- a/data/Data LA Study 20211208.xlsx
+++ b/data/Data LA Study 20211208.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhmockrin\Box\_Workspace\Proj_GitHub\la_wui_2112\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhmockrin\Box\_Workspace\Proj_GitHub22\La_wui\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28031BE0-B0A4-4562-B11B-267833EDA221}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EE6462-86DF-4D3C-AFC9-5072D6B4A0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_20211019_RForest" sheetId="10" r:id="rId1"/>
@@ -2351,12 +2351,12 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2671,14 +2671,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E470F27-90FE-46CE-BDA9-72D77DAC3EC2}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K1015"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2726,7 +2726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="55" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="55" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
         <v>461</v>
       </c>
@@ -2776,7 +2776,7 @@
       <c r="I3" s="54"/>
       <c r="J3" s="54"/>
     </row>
-    <row r="4" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="52">
         <v>2</v>
       </c>
@@ -2804,7 +2804,7 @@
       </c>
       <c r="J4" s="54"/>
     </row>
-    <row r="5" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="52">
         <v>3</v>
       </c>
@@ -2830,7 +2830,7 @@
       <c r="I5" s="54"/>
       <c r="J5" s="54"/>
     </row>
-    <row r="6" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="52">
         <v>4</v>
       </c>
@@ -2856,7 +2856,7 @@
       <c r="I6" s="54"/>
       <c r="J6" s="54"/>
     </row>
-    <row r="7" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="52">
         <v>5</v>
       </c>
@@ -2882,7 +2882,7 @@
       <c r="I7" s="54"/>
       <c r="J7" s="54"/>
     </row>
-    <row r="8" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="52">
         <v>6</v>
       </c>
@@ -2908,7 +2908,7 @@
       <c r="I8" s="54"/>
       <c r="J8" s="54"/>
     </row>
-    <row r="9" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="52">
         <v>7</v>
       </c>
@@ -2934,7 +2934,7 @@
       <c r="I9" s="54"/>
       <c r="J9" s="54"/>
     </row>
-    <row r="10" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="52">
         <v>8</v>
       </c>
@@ -2960,7 +2960,7 @@
       <c r="I10" s="54"/>
       <c r="J10" s="54"/>
     </row>
-    <row r="11" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="52">
         <v>9</v>
       </c>
@@ -2986,7 +2986,7 @@
       <c r="I11" s="54"/>
       <c r="J11" s="54"/>
     </row>
-    <row r="12" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="52">
         <v>10</v>
       </c>
@@ -3012,7 +3012,7 @@
       <c r="I12" s="54"/>
       <c r="J12" s="54"/>
     </row>
-    <row r="13" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="52">
         <v>11</v>
       </c>
@@ -3038,7 +3038,7 @@
       <c r="I13" s="54"/>
       <c r="J13" s="54"/>
     </row>
-    <row r="14" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="52">
         <v>12</v>
       </c>
@@ -3064,7 +3064,7 @@
       <c r="I14" s="54"/>
       <c r="J14" s="54"/>
     </row>
-    <row r="15" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="52">
         <v>13</v>
       </c>
@@ -3092,7 +3092,7 @@
       </c>
       <c r="J15" s="56"/>
     </row>
-    <row r="16" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="52">
         <v>14</v>
       </c>
@@ -3121,7 +3121,7 @@
       <c r="J16" s="54"/>
       <c r="K16" s="54"/>
     </row>
-    <row r="17" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="52">
         <v>15</v>
       </c>
@@ -3161,7 +3161,7 @@
       <c r="D18" s="57" t="s">
         <v>502</v>
       </c>
-      <c r="E18" s="66" t="s">
+      <c r="E18" s="63" t="s">
         <v>629</v>
       </c>
       <c r="F18" s="54" t="s">
@@ -3175,7 +3175,7 @@
       <c r="J18" s="54"/>
       <c r="K18" s="54"/>
     </row>
-    <row r="19" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="52">
         <v>16</v>
       </c>
@@ -3217,7 +3217,7 @@
       <c r="D20" s="57" t="s">
         <v>500</v>
       </c>
-      <c r="E20" s="66" t="s">
+      <c r="E20" s="63" t="s">
         <v>627</v>
       </c>
       <c r="F20" s="54" t="s">
@@ -3244,7 +3244,7 @@
       <c r="D21" s="57" t="s">
         <v>501</v>
       </c>
-      <c r="E21" s="66" t="s">
+      <c r="E21" s="63" t="s">
         <v>628</v>
       </c>
       <c r="F21" s="54" t="s">
@@ -3258,7 +3258,7 @@
       <c r="J21" s="54"/>
       <c r="K21" s="54"/>
     </row>
-    <row r="22" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="52">
         <v>20</v>
       </c>
@@ -3287,7 +3287,7 @@
       <c r="J22" s="54"/>
       <c r="K22" s="54"/>
     </row>
-    <row r="23" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="52">
         <v>21</v>
       </c>
@@ -3314,7 +3314,7 @@
       <c r="J23" s="54"/>
       <c r="K23" s="54"/>
     </row>
-    <row r="24" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="52">
         <v>22</v>
       </c>
@@ -3341,7 +3341,7 @@
       <c r="J24" s="54"/>
       <c r="K24" s="54"/>
     </row>
-    <row r="25" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="52">
         <v>23</v>
       </c>
@@ -3368,7 +3368,7 @@
       <c r="J25" s="54"/>
       <c r="K25" s="54"/>
     </row>
-    <row r="26" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="52">
         <v>24</v>
       </c>
@@ -3395,7 +3395,7 @@
       <c r="J26" s="54"/>
       <c r="K26" s="54"/>
     </row>
-    <row r="27" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="52">
         <v>25</v>
       </c>
@@ -3422,7 +3422,7 @@
       <c r="J27" s="54"/>
       <c r="K27" s="54"/>
     </row>
-    <row r="28" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="52">
         <v>26</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="52">
         <v>27</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="52">
         <v>28</v>
       </c>
@@ -3506,7 +3506,7 @@
       <c r="I30" s="54"/>
       <c r="J30" s="54"/>
     </row>
-    <row r="31" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="52">
         <v>29</v>
       </c>
@@ -3544,7 +3544,7 @@
       <c r="D32" s="57" t="s">
         <v>514</v>
       </c>
-      <c r="E32" s="66" t="s">
+      <c r="E32" s="63" t="s">
         <v>633</v>
       </c>
       <c r="F32" s="54" t="s">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="K32" s="54"/>
     </row>
-    <row r="33" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="52">
         <v>31</v>
       </c>
@@ -3588,7 +3588,7 @@
       </c>
       <c r="K33" s="54"/>
     </row>
-    <row r="34" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="52">
         <v>32</v>
       </c>
@@ -3613,7 +3613,7 @@
       <c r="H34" s="54"/>
       <c r="K34" s="54"/>
     </row>
-    <row r="35" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="52">
         <v>33</v>
       </c>
@@ -3638,7 +3638,7 @@
       <c r="H35" s="54"/>
       <c r="K35" s="54"/>
     </row>
-    <row r="36" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="52">
         <v>34</v>
       </c>
@@ -3663,7 +3663,7 @@
       <c r="H36" s="54"/>
       <c r="K36" s="54"/>
     </row>
-    <row r="37" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="52">
         <v>35</v>
       </c>
@@ -3688,7 +3688,7 @@
       <c r="H37" s="54"/>
       <c r="K37" s="54"/>
     </row>
-    <row r="38" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="52">
         <v>36</v>
       </c>
@@ -3713,7 +3713,7 @@
       <c r="H38" s="54"/>
       <c r="K38" s="54"/>
     </row>
-    <row r="39" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="52">
         <v>37</v>
       </c>
@@ -3738,7 +3738,7 @@
       <c r="H39" s="54"/>
       <c r="K39" s="54"/>
     </row>
-    <row r="40" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="52">
         <v>38</v>
       </c>
@@ -3763,7 +3763,7 @@
       <c r="H40" s="54"/>
       <c r="K40" s="54"/>
     </row>
-    <row r="41" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="52">
         <v>39</v>
       </c>
@@ -3788,7 +3788,7 @@
       <c r="H41" s="54"/>
       <c r="K41" s="54"/>
     </row>
-    <row r="42" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="52">
         <v>40</v>
       </c>
@@ -3813,7 +3813,7 @@
       <c r="H42" s="54"/>
       <c r="K42" s="54"/>
     </row>
-    <row r="43" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="52">
         <v>41</v>
       </c>
@@ -3838,7 +3838,7 @@
       <c r="H43" s="54"/>
       <c r="K43" s="54"/>
     </row>
-    <row r="44" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="52">
         <v>42</v>
       </c>
@@ -3864,7 +3864,7 @@
       <c r="J44" s="54"/>
       <c r="K44" s="54"/>
     </row>
-    <row r="45" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="52">
         <v>43</v>
       </c>
@@ -3891,7 +3891,7 @@
       <c r="J45" s="54"/>
       <c r="K45" s="54"/>
     </row>
-    <row r="46" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="52">
         <v>44</v>
       </c>
@@ -3918,7 +3918,7 @@
       <c r="J46" s="54"/>
       <c r="K46" s="54"/>
     </row>
-    <row r="47" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="52">
         <v>45</v>
       </c>
@@ -3945,7 +3945,7 @@
       <c r="J47" s="54"/>
       <c r="K47" s="54"/>
     </row>
-    <row r="48" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="52">
         <v>46</v>
       </c>
@@ -3972,7 +3972,7 @@
       <c r="J48" s="54"/>
       <c r="K48" s="54"/>
     </row>
-    <row r="49" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="52">
         <v>47</v>
       </c>
@@ -3999,7 +3999,7 @@
       <c r="J49" s="54"/>
       <c r="K49" s="54"/>
     </row>
-    <row r="50" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="52">
         <v>48</v>
       </c>
@@ -4026,7 +4026,7 @@
       <c r="J50" s="54"/>
       <c r="K50" s="54"/>
     </row>
-    <row r="51" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="52">
         <v>49</v>
       </c>
@@ -4053,7 +4053,7 @@
       <c r="J51" s="54"/>
       <c r="K51" s="54"/>
     </row>
-    <row r="52" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="52">
         <v>50</v>
       </c>
@@ -4080,7 +4080,7 @@
       <c r="J52" s="54"/>
       <c r="K52" s="54"/>
     </row>
-    <row r="53" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="52">
         <v>51</v>
       </c>
@@ -4107,7 +4107,7 @@
       <c r="J53" s="54"/>
       <c r="K53" s="54"/>
     </row>
-    <row r="54" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="52">
         <v>52</v>
       </c>
@@ -4134,7 +4134,7 @@
       <c r="J54" s="54"/>
       <c r="K54" s="54"/>
     </row>
-    <row r="55" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="52">
         <v>53</v>
       </c>
@@ -4161,7 +4161,7 @@
       <c r="J55" s="54"/>
       <c r="K55" s="54"/>
     </row>
-    <row r="56" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="52">
         <v>54</v>
       </c>
@@ -4188,7 +4188,7 @@
       <c r="J56" s="54"/>
       <c r="K56" s="54"/>
     </row>
-    <row r="57" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="52">
         <v>55</v>
       </c>
@@ -4215,7 +4215,7 @@
       <c r="J57" s="54"/>
       <c r="K57" s="54"/>
     </row>
-    <row r="58" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="52">
         <v>56</v>
       </c>
@@ -4242,7 +4242,7 @@
       <c r="J58" s="54"/>
       <c r="K58" s="54"/>
     </row>
-    <row r="59" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="52">
         <v>57</v>
       </c>
@@ -4269,7 +4269,7 @@
       <c r="J59" s="54"/>
       <c r="K59" s="54"/>
     </row>
-    <row r="60" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="52">
         <v>58</v>
       </c>
@@ -4296,7 +4296,7 @@
       <c r="J60" s="54"/>
       <c r="K60" s="54"/>
     </row>
-    <row r="61" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="52">
         <v>59</v>
       </c>
@@ -4323,7 +4323,7 @@
       <c r="J61" s="54"/>
       <c r="K61" s="54"/>
     </row>
-    <row r="62" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="52">
         <v>60</v>
       </c>
@@ -4350,7 +4350,7 @@
       <c r="J62" s="54"/>
       <c r="K62" s="54"/>
     </row>
-    <row r="63" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="52">
         <v>61</v>
       </c>
@@ -4377,7 +4377,7 @@
       <c r="J63" s="54"/>
       <c r="K63" s="54"/>
     </row>
-    <row r="64" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="52">
         <v>62</v>
       </c>
@@ -4417,7 +4417,7 @@
       <c r="D65" s="57" t="s">
         <v>547</v>
       </c>
-      <c r="E65" s="66" t="s">
+      <c r="E65" s="63" t="s">
         <v>630</v>
       </c>
       <c r="F65" s="54" t="s">
@@ -4443,7 +4443,7 @@
       <c r="D66" s="57" t="s">
         <v>548</v>
       </c>
-      <c r="E66" s="66" t="s">
+      <c r="E66" s="63" t="s">
         <v>587</v>
       </c>
       <c r="F66" s="54" t="s">
@@ -4471,7 +4471,7 @@
       <c r="D67" s="57" t="s">
         <v>549</v>
       </c>
-      <c r="E67" s="66" t="s">
+      <c r="E67" s="63" t="s">
         <v>631</v>
       </c>
       <c r="F67" s="54" t="s">
@@ -4497,7 +4497,7 @@
       <c r="D68" s="57" t="s">
         <v>550</v>
       </c>
-      <c r="E68" s="66" t="s">
+      <c r="E68" s="63" t="s">
         <v>632</v>
       </c>
       <c r="F68" s="54" t="s">
@@ -4509,7 +4509,7 @@
       <c r="H68" s="54"/>
       <c r="K68" s="54"/>
     </row>
-    <row r="69" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="52">
         <v>67</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="52">
         <v>68</v>
       </c>
@@ -4586,7 +4586,7 @@
       <c r="D71" s="55" t="s">
         <v>553</v>
       </c>
-      <c r="E71" s="66" t="s">
+      <c r="E71" s="63" t="s">
         <v>634</v>
       </c>
       <c r="F71" s="54" t="s">
@@ -4618,7 +4618,7 @@
       <c r="D72" s="55" t="s">
         <v>554</v>
       </c>
-      <c r="E72" s="66" t="s">
+      <c r="E72" s="63" t="s">
         <v>635</v>
       </c>
       <c r="F72" s="54" t="s">
@@ -4637,7 +4637,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="52">
         <v>71</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="52">
         <v>72</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="52" t="s">
         <v>461</v>
       </c>
@@ -4723,7 +4723,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="76" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="52" t="s">
         <v>461</v>
       </c>
@@ -4750,7 +4750,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="52" t="s">
         <v>461</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="55" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="52" t="s">
         <v>461</v>
       </c>
@@ -11330,14 +11330,7 @@
       <c r="E1015" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K78" xr:uid="{1E3BF0EA-EC3D-444C-9AE7-3F99453DC04F}">
-    <filterColumn colId="4">
-      <customFilters>
-        <customFilter val="*UNIT*"/>
-        <customFilter val="*NOTE*"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K78" xr:uid="{1E3BF0EA-EC3D-444C-9AE7-3F99453DC04F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A13:K21">
     <sortCondition ref="A13:A21"/>
   </sortState>
@@ -11375,15 +11368,15 @@
     <row r="1" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="38"/>
       <c r="B1" s="38"/>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="64" t="s">
         <v>260</v>
       </c>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65" t="s">
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="66" t="s">
         <v>261</v>
       </c>
-      <c r="G1" s="64"/>
+      <c r="G1" s="65"/>
     </row>
     <row r="2" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
@@ -30466,7 +30459,7 @@
   </sheetPr>
   <dimension ref="A1:AE1082"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>